<commit_message>
More relavant name for localization
</commit_message>
<xml_diff>
--- a/StringLocalization.xlsx
+++ b/StringLocalization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyg/Work/Projects/localizer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyg/Work/Projects/fast-locale/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -242,18 +242,6 @@
     <t>ro</t>
   </si>
   <si>
-    <t xml:space="preserve">RA_You_are_not_LoggedIn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RA_OK </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RA_Cancel </t>
-  </si>
-  <si>
-    <t>RA_Warning</t>
-  </si>
-  <si>
     <t>You are not Logged In. Please go to Settings and Log In</t>
   </si>
   <si>
@@ -1630,6 +1618,18 @@
   </si>
   <si>
     <t>zh-Hant-TW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You_are_not_LoggedIn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel </t>
+  </si>
+  <si>
+    <t>Warning</t>
   </si>
 </sst>
 </file>
@@ -3079,7 +3079,7 @@
   <dimension ref="A1:IG26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="83" zoomScaleNormal="97" zoomScalePageLayoutView="97" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="39.375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3234,16 +3234,16 @@
         <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>40</v>
@@ -3252,7 +3252,7 @@
         <v>41</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>42</v>
@@ -3288,7 +3288,7 @@
         <v>51</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>52</v>
@@ -3352,121 +3352,121 @@
     </row>
     <row r="3" spans="1:241" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="C3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="J3" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="T3" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="U3" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="V3" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="W3" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="X3" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y3" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z3" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="O3" s="18" t="s">
+      <c r="AA3" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB3" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC3" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="P3" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="R3" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="S3" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="T3" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="U3" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="V3" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="W3" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="X3" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y3" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z3" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA3" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB3" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="AC3" s="18" t="s">
-        <v>139</v>
-      </c>
       <c r="AD3" s="18" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="AE3" s="18" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AF3" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="AG3" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH3" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="AI3" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="AJ3" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK3" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL3" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="AG3" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH3" s="18" t="s">
+      <c r="AM3" s="18" t="s">
         <v>172</v>
-      </c>
-      <c r="AI3" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="AJ3" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="AK3" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="AL3" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="AM3" s="18" t="s">
-        <v>176</v>
       </c>
       <c r="AN3" s="13"/>
       <c r="AO3" s="13"/>
@@ -3476,121 +3476,121 @@
     </row>
     <row r="4" spans="1:241" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="C4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>80</v>
-      </c>
       <c r="J4" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="N4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="O4" s="18" t="s">
+      <c r="P4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="S4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="T4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="U4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="V4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y4" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z4" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB4" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC4" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="P4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="R4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="S4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="T4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="U4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="V4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="W4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="X4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y4" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z4" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB4" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="AC4" s="18" t="s">
-        <v>140</v>
-      </c>
       <c r="AD4" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AE4" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AF4" s="18" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="AG4" s="18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="AH4" s="18" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="AI4" s="18" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="AJ4" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AK4" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AL4" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AM4" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AN4" s="14"/>
       <c r="AO4" s="14"/>
@@ -3797,121 +3797,121 @@
     </row>
     <row r="5" spans="1:241" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="C5" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="J5" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R5" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="S5" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="T5" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="U5" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="V5" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="W5" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="X5" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y5" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5" s="18" t="s">
+      <c r="Z5" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA5" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB5" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC5" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="P5" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q5" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="R5" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="S5" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="T5" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="U5" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="V5" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="W5" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="X5" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y5" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z5" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA5" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB5" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC5" s="18" t="s">
-        <v>141</v>
-      </c>
       <c r="AD5" s="18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AE5" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF5" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="AF5" s="18" t="s">
-        <v>168</v>
-      </c>
       <c r="AG5" s="18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AH5" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="AI5" s="18" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="AJ5" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AK5" s="18" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AL5" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="AM5" s="18" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AN5" s="13"/>
       <c r="AO5" s="13"/>
@@ -3921,121 +3921,121 @@
     </row>
     <row r="6" spans="1:241" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="J6" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="O6" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="T6" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="U6" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="V6" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="W6" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="X6" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y6" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="O6" s="18" t="s">
+      <c r="Z6" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA6" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC6" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="P6" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q6" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="R6" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="S6" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="T6" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="U6" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="V6" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="W6" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="X6" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y6" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z6" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA6" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB6" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC6" s="18" t="s">
-        <v>142</v>
-      </c>
       <c r="AD6" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AE6" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF6" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="AF6" s="18" t="s">
-        <v>169</v>
-      </c>
       <c r="AG6" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="AH6" s="18" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AI6" s="18" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AJ6" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AK6" s="18" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AL6" s="18" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM6" s="18" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="AN6" s="13"/>
       <c r="AO6" s="13"/>

</xml_diff>